<commit_message>
#1335 working without knowing edge cases / submitting
</commit_message>
<xml_diff>
--- a/1335. Minimum Difficulty of a Job Schedule/Whiteboards/Solution.xlsx
+++ b/1335. Minimum Difficulty of a Job Schedule/Whiteboards/Solution.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Portalz\Desktop\Small Projects\LeetCode\1335. Minimum Difficulty of a Job Schedule\Whiteboards\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26F85DBC-47E6-4DC3-B9DB-EC7C13087CC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA7B38F6-8ACD-4E47-AE3B-7D03679B094B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{756CC0B2-6BE7-4EF6-9EEE-182F71A93026}"/>
+    <workbookView xWindow="10395" yWindow="1995" windowWidth="18315" windowHeight="11385" xr2:uid="{756CC0B2-6BE7-4EF6-9EEE-182F71A93026}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -465,10 +465,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79CF585D-CE06-44D4-80AA-070156E711E0}">
-  <dimension ref="F7:AM149"/>
+  <dimension ref="E7:AM164"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A134" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="Y144" sqref="Y144"/>
+    <sheetView tabSelected="1" topLeftCell="A150" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L166" sqref="L166"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.7109375" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2397,7 +2397,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="129" spans="10:39" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="5:39" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="AA129" s="1">
         <v>1</v>
       </c>
@@ -2432,7 +2432,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="130" spans="10:39" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="5:39" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="AA130" s="1">
         <v>100</v>
       </c>
@@ -2467,7 +2467,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="132" spans="10:39" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="5:39" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="R132" s="1">
         <v>5</v>
       </c>
@@ -2487,7 +2487,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="134" spans="10:39" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="5:39" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="AA134" s="1">
         <v>1</v>
       </c>
@@ -2525,7 +2525,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="135" spans="10:39" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="5:39" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="R135" s="1">
         <v>5</v>
       </c>
@@ -2542,7 +2542,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="136" spans="10:39" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="5:39" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="AA136" s="1">
         <v>1</v>
       </c>
@@ -2577,7 +2577,28 @@
         <v>100</v>
       </c>
     </row>
-    <row r="137" spans="10:39" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="5:39" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E137" s="1">
+        <v>0</v>
+      </c>
+      <c r="F137" s="1">
+        <v>1</v>
+      </c>
+      <c r="G137" s="1">
+        <v>2</v>
+      </c>
+      <c r="H137" s="1">
+        <v>3</v>
+      </c>
+      <c r="I137" s="1">
+        <v>4</v>
+      </c>
+      <c r="J137" s="1">
+        <v>5</v>
+      </c>
+      <c r="K137" s="1">
+        <v>6</v>
+      </c>
       <c r="AA137" s="1">
         <v>1</v>
       </c>
@@ -2612,7 +2633,30 @@
         <v>1</v>
       </c>
     </row>
-    <row r="139" spans="10:39" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="5:39" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E138" s="1">
+        <v>10</v>
+      </c>
+      <c r="F138" s="1">
+        <v>5</v>
+      </c>
+      <c r="G138" s="1">
+        <v>2</v>
+      </c>
+      <c r="H138" s="1">
+        <v>4</v>
+      </c>
+      <c r="I138" s="1">
+        <v>8</v>
+      </c>
+      <c r="J138" s="1">
+        <v>1</v>
+      </c>
+      <c r="K138" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="139" spans="5:39" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="Y139" s="1">
         <v>1</v>
       </c>
@@ -2650,7 +2694,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="140" spans="10:39" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="5:39" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J140" s="1">
         <v>1</v>
       </c>
@@ -2658,7 +2702,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="141" spans="10:39" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="5:39" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J141" s="1">
         <v>1</v>
       </c>
@@ -2699,7 +2743,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="142" spans="10:39" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="5:39" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J142" s="1">
         <v>1</v>
       </c>
@@ -2743,7 +2787,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="143" spans="10:39" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="5:39" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J143" s="1">
         <v>100</v>
       </c>
@@ -2760,7 +2804,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="144" spans="10:39" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="5:39" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J144" s="1">
         <v>1</v>
       </c>
@@ -2832,6 +2876,63 @@
       </c>
       <c r="AF149" s="1">
         <v>1</v>
+      </c>
+    </row>
+    <row r="161" spans="5:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E161" s="1">
+        <v>0</v>
+      </c>
+      <c r="F161" s="1">
+        <v>1</v>
+      </c>
+      <c r="G161" s="1">
+        <v>2</v>
+      </c>
+      <c r="H161" s="1">
+        <v>3</v>
+      </c>
+      <c r="I161" s="1">
+        <v>4</v>
+      </c>
+      <c r="K161" s="1">
+        <v>5</v>
+      </c>
+      <c r="M161" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="162" spans="5:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E162" s="1">
+        <v>10</v>
+      </c>
+      <c r="F162" s="1">
+        <v>5</v>
+      </c>
+      <c r="G162" s="1">
+        <v>2</v>
+      </c>
+      <c r="H162" s="1">
+        <v>4</v>
+      </c>
+      <c r="I162" s="1">
+        <v>8</v>
+      </c>
+      <c r="K162" s="1">
+        <v>1</v>
+      </c>
+      <c r="M162" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="164" spans="5:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F164" s="1">
+        <v>10</v>
+      </c>
+      <c r="K164" s="1">
+        <v>1</v>
+      </c>
+      <c r="M164" s="1">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>